<commit_message>
mean and median order corrected
</commit_message>
<xml_diff>
--- a/Evaluation/MARC_PAPER/Statistical_output/ArCoMo1400/ArCoMo1400_statistical_results_area_difference_comparison.xlsx
+++ b/Evaluation/MARC_PAPER/Statistical_output/ArCoMo1400/ArCoMo1400_statistical_results_area_difference_comparison.xlsx
@@ -446,12 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Mean Absolute Error</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Median Absolute Error</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Mean Absolute Error</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">

</xml_diff>